<commit_message>
Se agregan escenarios de pruebas manuales exploratorias
</commit_message>
<xml_diff>
--- a/Inventario Pruebas Exploratorias.xlsx
+++ b/Inventario Pruebas Exploratorias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acastiblanco/Documents/Learning/MISO/Pruebas automatizadas de software/Entrega 5/E2E-Ghost-Kraken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC08850-F79D-FB41-8004-2DEA100FE970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E788FC61-9495-6C4F-8068-E9C949E734A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36460" yWindow="4940" windowWidth="36480" windowHeight="19340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1350,7 +1350,7 @@
   <dimension ref="B1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:J7"/>
+      <selection activeCell="C6" sqref="C6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>